<commit_message>
stage2 local-label statistics correction
</commit_message>
<xml_diff>
--- a/res/标记数据统计.xlsx
+++ b/res/标记数据统计.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="15550" windowHeight="7340" tabRatio="993" activeTab="3"/>
+    <workbookView windowWidth="19100" windowHeight="8690" tabRatio="993" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Stage1" sheetId="1" r:id="rId1"/>
@@ -1084,11 +1084,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1217,30 +1217,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1260,17 +1251,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1283,59 +1274,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1357,11 +1296,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1374,7 +1374,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,13 +1416,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1404,7 +1446,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1416,19 +1512,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1446,31 +1530,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1483,78 +1555,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1660,6 +1660,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1671,6 +1686,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1699,6 +1725,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1713,182 +1748,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="24" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="24" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="23" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="23" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2023,9 +2023,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2393,131 +2390,131 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.6272727272727" style="61"/>
-    <col min="2" max="2" width="9" style="61" customWidth="1"/>
-    <col min="3" max="3" width="9" style="61"/>
-    <col min="4" max="4" width="9" style="57"/>
-    <col min="5" max="1025" width="9" style="61"/>
+    <col min="1" max="1" width="12.6272727272727" style="60"/>
+    <col min="2" max="2" width="9" style="60" customWidth="1"/>
+    <col min="3" max="3" width="9" style="60"/>
+    <col min="4" max="4" width="9" style="56"/>
+    <col min="5" max="1025" width="9" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="63" t="s">
+      <c r="N1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="63" t="s">
+      <c r="O1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="P1" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="63" t="s">
+      <c r="Q1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="63" t="s">
+      <c r="S1" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="63" t="s">
+      <c r="U1" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="63" t="s">
+      <c r="V1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="63" t="s">
+      <c r="W1" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="61" t="s">
+      <c r="X1" s="60" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" ht="14.5" spans="1:1025">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="60">
+      <c r="D2" s="59">
         <f t="shared" ref="D2:D20" si="0">SUM(F2:S2)</f>
         <v>7248</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="61">
+      <c r="E2" s="63"/>
+      <c r="F2" s="60">
         <v>1611</v>
       </c>
-      <c r="G2" s="61">
+      <c r="G2" s="60">
         <v>7</v>
       </c>
-      <c r="H2" s="61">
+      <c r="H2" s="60">
         <v>3707</v>
       </c>
-      <c r="I2" s="61">
+      <c r="I2" s="60">
         <v>427</v>
       </c>
-      <c r="J2" s="61">
+      <c r="J2" s="60">
         <v>307</v>
       </c>
-      <c r="K2" s="61">
+      <c r="K2" s="60">
         <v>164</v>
       </c>
-      <c r="L2" s="61">
-        <v>0</v>
-      </c>
-      <c r="M2" s="61">
+      <c r="L2" s="60">
+        <v>0</v>
+      </c>
+      <c r="M2" s="60">
         <v>322</v>
       </c>
-      <c r="N2" s="61">
+      <c r="N2" s="60">
         <v>152</v>
       </c>
-      <c r="O2" s="61">
+      <c r="O2" s="60">
         <v>274</v>
       </c>
-      <c r="P2" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="61">
+      <c r="P2" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="60">
         <v>66</v>
       </c>
-      <c r="R2" s="61">
+      <c r="R2" s="60">
         <v>196</v>
       </c>
-      <c r="S2" s="61">
+      <c r="S2" s="60">
         <v>15</v>
       </c>
       <c r="T2"/>
@@ -3533,57 +3530,57 @@
       <c r="AMK2"/>
     </row>
     <row r="3" ht="14.5" spans="1:1025">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="60">
+      <c r="D3" s="59">
         <f t="shared" si="0"/>
         <v>9399</v>
       </c>
-      <c r="F3" s="61">
-        <v>0</v>
-      </c>
-      <c r="G3" s="61">
-        <v>0</v>
-      </c>
-      <c r="H3" s="61">
+      <c r="F3" s="60">
+        <v>0</v>
+      </c>
+      <c r="G3" s="60">
+        <v>0</v>
+      </c>
+      <c r="H3" s="60">
         <v>5812</v>
       </c>
-      <c r="I3" s="61">
+      <c r="I3" s="60">
         <v>1551</v>
       </c>
-      <c r="J3" s="61">
-        <v>0</v>
-      </c>
-      <c r="K3" s="61">
-        <v>0</v>
-      </c>
-      <c r="L3" s="61">
+      <c r="J3" s="60">
+        <v>0</v>
+      </c>
+      <c r="K3" s="60">
+        <v>0</v>
+      </c>
+      <c r="L3" s="60">
         <v>732</v>
       </c>
-      <c r="M3" s="61">
-        <v>0</v>
-      </c>
-      <c r="N3" s="61">
-        <v>0</v>
-      </c>
-      <c r="O3" s="61">
+      <c r="M3" s="60">
+        <v>0</v>
+      </c>
+      <c r="N3" s="60">
+        <v>0</v>
+      </c>
+      <c r="O3" s="60">
         <v>56</v>
       </c>
-      <c r="P3" s="61">
+      <c r="P3" s="60">
         <v>1058</v>
       </c>
-      <c r="Q3" s="61">
-        <v>0</v>
-      </c>
-      <c r="R3" s="61">
+      <c r="Q3" s="60">
+        <v>0</v>
+      </c>
+      <c r="R3" s="60">
         <v>190</v>
       </c>
-      <c r="S3" s="61">
+      <c r="S3" s="60">
         <v>0</v>
       </c>
       <c r="T3"/>
@@ -4593,57 +4590,57 @@
       <c r="AMK3"/>
     </row>
     <row r="4" ht="14.5" spans="1:1025">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="56" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="59">
         <f t="shared" si="0"/>
         <v>3504</v>
       </c>
-      <c r="F4" s="61">
-        <v>0</v>
-      </c>
-      <c r="G4" s="61">
-        <v>0</v>
-      </c>
-      <c r="H4" s="61">
+      <c r="F4" s="60">
+        <v>0</v>
+      </c>
+      <c r="G4" s="60">
+        <v>0</v>
+      </c>
+      <c r="H4" s="60">
         <v>299</v>
       </c>
-      <c r="I4" s="61">
+      <c r="I4" s="60">
         <v>219</v>
       </c>
-      <c r="J4" s="61">
-        <v>0</v>
-      </c>
-      <c r="K4" s="61">
-        <v>0</v>
-      </c>
-      <c r="L4" s="61">
+      <c r="J4" s="60">
+        <v>0</v>
+      </c>
+      <c r="K4" s="60">
+        <v>0</v>
+      </c>
+      <c r="L4" s="60">
         <v>2670</v>
       </c>
-      <c r="M4" s="61">
-        <v>0</v>
-      </c>
-      <c r="N4" s="61">
-        <v>0</v>
-      </c>
-      <c r="O4" s="61">
-        <v>0</v>
-      </c>
-      <c r="P4" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="61">
-        <v>0</v>
-      </c>
-      <c r="R4" s="61">
+      <c r="M4" s="60">
+        <v>0</v>
+      </c>
+      <c r="N4" s="60">
+        <v>0</v>
+      </c>
+      <c r="O4" s="60">
+        <v>0</v>
+      </c>
+      <c r="P4" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="60">
+        <v>0</v>
+      </c>
+      <c r="R4" s="60">
         <v>286</v>
       </c>
-      <c r="S4" s="61">
+      <c r="S4" s="60">
         <v>30</v>
       </c>
       <c r="T4"/>
@@ -5653,57 +5650,57 @@
       <c r="AMK4"/>
     </row>
     <row r="5" ht="14.5" spans="1:1025">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="56" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="59">
         <f t="shared" si="0"/>
         <v>4580</v>
       </c>
-      <c r="F5" s="61">
+      <c r="F5" s="60">
         <v>1566</v>
       </c>
-      <c r="G5" s="61">
-        <v>0</v>
-      </c>
-      <c r="H5" s="61">
+      <c r="G5" s="60">
+        <v>0</v>
+      </c>
+      <c r="H5" s="60">
         <v>290</v>
       </c>
-      <c r="I5" s="61">
+      <c r="I5" s="60">
         <v>160</v>
       </c>
-      <c r="J5" s="61">
+      <c r="J5" s="60">
         <v>84</v>
       </c>
-      <c r="K5" s="61">
+      <c r="K5" s="60">
         <v>306</v>
       </c>
-      <c r="L5" s="61">
-        <v>0</v>
-      </c>
-      <c r="M5" s="61">
+      <c r="L5" s="60">
+        <v>0</v>
+      </c>
+      <c r="M5" s="60">
         <v>73</v>
       </c>
-      <c r="N5" s="61">
+      <c r="N5" s="60">
         <v>453</v>
       </c>
-      <c r="O5" s="61">
+      <c r="O5" s="60">
         <v>288</v>
       </c>
-      <c r="P5" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="61">
+      <c r="P5" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="60">
         <v>1356</v>
       </c>
-      <c r="R5" s="61">
-        <v>0</v>
-      </c>
-      <c r="S5" s="61">
+      <c r="R5" s="60">
+        <v>0</v>
+      </c>
+      <c r="S5" s="60">
         <v>4</v>
       </c>
       <c r="T5"/>
@@ -6713,57 +6710,57 @@
       <c r="AMK5"/>
     </row>
     <row r="6" ht="14.5" spans="1:1025">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="56" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="59">
         <f t="shared" si="0"/>
         <v>1397</v>
       </c>
-      <c r="F6" s="61">
+      <c r="F6" s="60">
         <v>80</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="60">
         <v>1</v>
       </c>
-      <c r="H6" s="61">
+      <c r="H6" s="60">
         <v>167</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="60">
         <v>8</v>
       </c>
-      <c r="J6" s="61">
-        <v>0</v>
-      </c>
-      <c r="K6" s="61">
+      <c r="J6" s="60">
+        <v>0</v>
+      </c>
+      <c r="K6" s="60">
         <v>843</v>
       </c>
-      <c r="L6" s="61">
-        <v>0</v>
-      </c>
-      <c r="M6" s="61">
-        <v>0</v>
-      </c>
-      <c r="N6" s="61">
+      <c r="L6" s="60">
+        <v>0</v>
+      </c>
+      <c r="M6" s="60">
+        <v>0</v>
+      </c>
+      <c r="N6" s="60">
         <v>239</v>
       </c>
-      <c r="O6" s="61">
+      <c r="O6" s="60">
         <v>33</v>
       </c>
-      <c r="P6" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="61">
+      <c r="P6" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="60">
         <v>15</v>
       </c>
-      <c r="R6" s="61">
+      <c r="R6" s="60">
         <v>11</v>
       </c>
-      <c r="S6" s="61">
+      <c r="S6" s="60">
         <v>0</v>
       </c>
       <c r="T6"/>
@@ -7773,57 +7770,57 @@
       <c r="AMK6"/>
     </row>
     <row r="7" ht="14.5" spans="1:1025">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="56" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="59">
         <f t="shared" si="0"/>
         <v>7328</v>
       </c>
-      <c r="F7" s="61">
-        <v>0</v>
-      </c>
-      <c r="G7" s="61">
+      <c r="F7" s="60">
+        <v>0</v>
+      </c>
+      <c r="G7" s="60">
         <v>758</v>
       </c>
-      <c r="H7" s="61">
+      <c r="H7" s="60">
         <v>4</v>
       </c>
-      <c r="I7" s="61">
+      <c r="I7" s="60">
         <v>3</v>
       </c>
-      <c r="J7" s="61">
+      <c r="J7" s="60">
         <v>2107</v>
       </c>
-      <c r="K7" s="61">
+      <c r="K7" s="60">
         <v>1685</v>
       </c>
-      <c r="L7" s="61">
-        <v>0</v>
-      </c>
-      <c r="M7" s="61">
+      <c r="L7" s="60">
+        <v>0</v>
+      </c>
+      <c r="M7" s="60">
         <v>566</v>
       </c>
-      <c r="N7" s="61">
+      <c r="N7" s="60">
         <v>17</v>
       </c>
-      <c r="O7" s="61">
+      <c r="O7" s="60">
         <v>2147</v>
       </c>
-      <c r="P7" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="61">
-        <v>0</v>
-      </c>
-      <c r="R7" s="61">
+      <c r="P7" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="60">
+        <v>0</v>
+      </c>
+      <c r="R7" s="60">
         <v>41</v>
       </c>
-      <c r="S7" s="61">
+      <c r="S7" s="60">
         <v>0</v>
       </c>
       <c r="T7"/>
@@ -8833,57 +8830,57 @@
       <c r="AMK7"/>
     </row>
     <row r="8" ht="14.5" spans="1:1025">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="56" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="59">
         <f t="shared" si="0"/>
         <v>5538</v>
       </c>
-      <c r="F8" s="61">
+      <c r="F8" s="60">
         <v>134</v>
       </c>
-      <c r="G8" s="61">
+      <c r="G8" s="60">
         <v>479</v>
       </c>
-      <c r="H8" s="61">
+      <c r="H8" s="60">
         <v>180</v>
       </c>
-      <c r="I8" s="61">
+      <c r="I8" s="60">
         <v>38</v>
       </c>
-      <c r="J8" s="61">
+      <c r="J8" s="60">
         <v>557</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="60">
         <v>1146</v>
       </c>
-      <c r="L8" s="61">
+      <c r="L8" s="60">
         <v>33</v>
       </c>
-      <c r="M8" s="61">
+      <c r="M8" s="60">
         <v>659</v>
       </c>
-      <c r="N8" s="61">
+      <c r="N8" s="60">
         <v>363</v>
       </c>
-      <c r="O8" s="61">
+      <c r="O8" s="60">
         <v>1496</v>
       </c>
-      <c r="P8" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="61">
+      <c r="P8" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="60">
         <v>58</v>
       </c>
-      <c r="R8" s="61">
+      <c r="R8" s="60">
         <v>391</v>
       </c>
-      <c r="S8" s="61">
+      <c r="S8" s="60">
         <v>4</v>
       </c>
       <c r="T8"/>
@@ -9893,57 +9890,57 @@
       <c r="AMK8"/>
     </row>
     <row r="9" ht="14.5" spans="1:1025">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="56" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="59">
         <f t="shared" si="0"/>
         <v>1156</v>
       </c>
-      <c r="F9" s="61">
+      <c r="F9" s="60">
         <v>1</v>
       </c>
-      <c r="G9" s="61">
-        <v>0</v>
-      </c>
-      <c r="H9" s="61">
+      <c r="G9" s="60">
+        <v>0</v>
+      </c>
+      <c r="H9" s="60">
         <v>5</v>
       </c>
-      <c r="I9" s="61">
+      <c r="I9" s="60">
         <v>3</v>
       </c>
-      <c r="J9" s="61">
-        <v>0</v>
-      </c>
-      <c r="K9" s="61">
+      <c r="J9" s="60">
+        <v>0</v>
+      </c>
+      <c r="K9" s="60">
         <v>1</v>
       </c>
-      <c r="L9" s="61">
-        <v>0</v>
-      </c>
-      <c r="M9" s="61">
-        <v>0</v>
-      </c>
-      <c r="N9" s="61">
-        <v>0</v>
-      </c>
-      <c r="O9" s="61">
-        <v>0</v>
-      </c>
-      <c r="P9" s="61">
+      <c r="L9" s="60">
+        <v>0</v>
+      </c>
+      <c r="M9" s="60">
+        <v>0</v>
+      </c>
+      <c r="N9" s="60">
+        <v>0</v>
+      </c>
+      <c r="O9" s="60">
+        <v>0</v>
+      </c>
+      <c r="P9" s="60">
         <v>1146</v>
       </c>
-      <c r="Q9" s="61">
-        <v>0</v>
-      </c>
-      <c r="R9" s="61">
-        <v>0</v>
-      </c>
-      <c r="S9" s="61">
+      <c r="Q9" s="60">
+        <v>0</v>
+      </c>
+      <c r="R9" s="60">
+        <v>0</v>
+      </c>
+      <c r="S9" s="60">
         <v>0</v>
       </c>
       <c r="T9"/>
@@ -10953,57 +10950,57 @@
       <c r="AMK9"/>
     </row>
     <row r="10" ht="14.5" spans="1:1025">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="56" t="s">
+      <c r="B10" s="63"/>
+      <c r="C10" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="59">
         <f t="shared" si="0"/>
         <v>2846</v>
       </c>
-      <c r="F10" s="61">
+      <c r="F10" s="60">
         <v>539</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="60">
         <v>605</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="60">
         <v>325</v>
       </c>
-      <c r="I10" s="61">
+      <c r="I10" s="60">
         <v>78</v>
       </c>
-      <c r="J10" s="61">
+      <c r="J10" s="60">
         <v>90</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="60">
         <v>294</v>
       </c>
-      <c r="L10" s="61">
-        <v>0</v>
-      </c>
-      <c r="M10" s="61">
+      <c r="L10" s="60">
+        <v>0</v>
+      </c>
+      <c r="M10" s="60">
         <v>17</v>
       </c>
-      <c r="N10" s="61">
+      <c r="N10" s="60">
         <v>76</v>
       </c>
-      <c r="O10" s="61">
+      <c r="O10" s="60">
         <v>177</v>
       </c>
-      <c r="P10" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="61">
+      <c r="P10" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="60">
         <v>597</v>
       </c>
-      <c r="R10" s="61">
+      <c r="R10" s="60">
         <v>40</v>
       </c>
-      <c r="S10" s="61">
+      <c r="S10" s="60">
         <v>8</v>
       </c>
       <c r="T10"/>
@@ -12013,57 +12010,57 @@
       <c r="AMK10"/>
     </row>
     <row r="11" ht="14.5" spans="1:1025">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="56" t="s">
+      <c r="B11" s="65"/>
+      <c r="C11" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="59">
         <f t="shared" si="0"/>
         <v>371</v>
       </c>
-      <c r="F11" s="61">
-        <v>0</v>
-      </c>
-      <c r="G11" s="61">
-        <v>0</v>
-      </c>
-      <c r="H11" s="61">
-        <v>0</v>
-      </c>
-      <c r="I11" s="61">
-        <v>0</v>
-      </c>
-      <c r="J11" s="61">
-        <v>0</v>
-      </c>
-      <c r="K11" s="61">
+      <c r="F11" s="60">
+        <v>0</v>
+      </c>
+      <c r="G11" s="60">
+        <v>0</v>
+      </c>
+      <c r="H11" s="60">
+        <v>0</v>
+      </c>
+      <c r="I11" s="60">
+        <v>0</v>
+      </c>
+      <c r="J11" s="60">
+        <v>0</v>
+      </c>
+      <c r="K11" s="60">
         <v>1</v>
       </c>
-      <c r="L11" s="61">
-        <v>0</v>
-      </c>
-      <c r="M11" s="61">
-        <v>0</v>
-      </c>
-      <c r="N11" s="61">
-        <v>0</v>
-      </c>
-      <c r="O11" s="61">
-        <v>0</v>
-      </c>
-      <c r="P11" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="61">
-        <v>0</v>
-      </c>
-      <c r="R11" s="61">
-        <v>0</v>
-      </c>
-      <c r="S11" s="61">
+      <c r="L11" s="60">
+        <v>0</v>
+      </c>
+      <c r="M11" s="60">
+        <v>0</v>
+      </c>
+      <c r="N11" s="60">
+        <v>0</v>
+      </c>
+      <c r="O11" s="60">
+        <v>0</v>
+      </c>
+      <c r="P11" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="60">
+        <v>0</v>
+      </c>
+      <c r="R11" s="60">
+        <v>0</v>
+      </c>
+      <c r="S11" s="60">
         <v>370</v>
       </c>
       <c r="T11"/>
@@ -13073,57 +13070,57 @@
       <c r="AMK11"/>
     </row>
     <row r="12" ht="14.5" spans="1:1025">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="56" t="s">
+      <c r="B12" s="63"/>
+      <c r="C12" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="59">
         <f t="shared" si="0"/>
         <v>242</v>
       </c>
-      <c r="F12" s="61">
+      <c r="F12" s="60">
         <v>1</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="60">
         <v>30</v>
       </c>
-      <c r="H12" s="61">
+      <c r="H12" s="60">
         <v>3</v>
       </c>
-      <c r="I12" s="61">
+      <c r="I12" s="60">
         <v>1</v>
       </c>
-      <c r="J12" s="61">
-        <v>0</v>
-      </c>
-      <c r="K12" s="61">
-        <v>0</v>
-      </c>
-      <c r="L12" s="61">
-        <v>0</v>
-      </c>
-      <c r="M12" s="61">
-        <v>0</v>
-      </c>
-      <c r="N12" s="61">
+      <c r="J12" s="60">
+        <v>0</v>
+      </c>
+      <c r="K12" s="60">
+        <v>0</v>
+      </c>
+      <c r="L12" s="60">
+        <v>0</v>
+      </c>
+      <c r="M12" s="60">
+        <v>0</v>
+      </c>
+      <c r="N12" s="60">
         <v>188</v>
       </c>
-      <c r="O12" s="61">
+      <c r="O12" s="60">
         <v>4</v>
       </c>
-      <c r="P12" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="61">
-        <v>0</v>
-      </c>
-      <c r="R12" s="61">
-        <v>0</v>
-      </c>
-      <c r="S12" s="61">
+      <c r="P12" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="60">
+        <v>0</v>
+      </c>
+      <c r="R12" s="60">
+        <v>0</v>
+      </c>
+      <c r="S12" s="60">
         <v>15</v>
       </c>
       <c r="T12"/>
@@ -14133,57 +14130,57 @@
       <c r="AMK12"/>
     </row>
     <row r="13" ht="14.5" spans="1:1025">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="56" t="s">
+      <c r="B13" s="65"/>
+      <c r="C13" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="60">
+      <c r="D13" s="59">
         <f t="shared" si="0"/>
         <v>509</v>
       </c>
-      <c r="F13" s="61">
-        <v>0</v>
-      </c>
-      <c r="G13" s="61">
-        <v>0</v>
-      </c>
-      <c r="H13" s="61">
-        <v>0</v>
-      </c>
-      <c r="I13" s="61">
-        <v>0</v>
-      </c>
-      <c r="J13" s="61">
-        <v>0</v>
-      </c>
-      <c r="K13" s="61">
-        <v>0</v>
-      </c>
-      <c r="L13" s="61">
-        <v>0</v>
-      </c>
-      <c r="M13" s="61">
-        <v>0</v>
-      </c>
-      <c r="N13" s="61">
-        <v>0</v>
-      </c>
-      <c r="O13" s="61">
-        <v>0</v>
-      </c>
-      <c r="P13" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="61">
-        <v>0</v>
-      </c>
-      <c r="R13" s="61">
+      <c r="F13" s="60">
+        <v>0</v>
+      </c>
+      <c r="G13" s="60">
+        <v>0</v>
+      </c>
+      <c r="H13" s="60">
+        <v>0</v>
+      </c>
+      <c r="I13" s="60">
+        <v>0</v>
+      </c>
+      <c r="J13" s="60">
+        <v>0</v>
+      </c>
+      <c r="K13" s="60">
+        <v>0</v>
+      </c>
+      <c r="L13" s="60">
+        <v>0</v>
+      </c>
+      <c r="M13" s="60">
+        <v>0</v>
+      </c>
+      <c r="N13" s="60">
+        <v>0</v>
+      </c>
+      <c r="O13" s="60">
+        <v>0</v>
+      </c>
+      <c r="P13" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="60">
+        <v>0</v>
+      </c>
+      <c r="R13" s="60">
         <v>360</v>
       </c>
-      <c r="S13" s="61">
+      <c r="S13" s="60">
         <v>149</v>
       </c>
       <c r="T13"/>
@@ -15193,57 +15190,57 @@
       <c r="AMK13"/>
     </row>
     <row r="14" ht="14.5" spans="1:1025">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="56" t="s">
+      <c r="B14" s="65"/>
+      <c r="C14" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="60">
+      <c r="D14" s="59">
         <f t="shared" si="0"/>
         <v>253</v>
       </c>
-      <c r="F14" s="61">
-        <v>0</v>
-      </c>
-      <c r="G14" s="61">
+      <c r="F14" s="60">
+        <v>0</v>
+      </c>
+      <c r="G14" s="60">
         <v>53</v>
       </c>
-      <c r="H14" s="61">
-        <v>0</v>
-      </c>
-      <c r="I14" s="61">
-        <v>0</v>
-      </c>
-      <c r="J14" s="61">
-        <v>0</v>
-      </c>
-      <c r="K14" s="61">
-        <v>0</v>
-      </c>
-      <c r="L14" s="61">
-        <v>0</v>
-      </c>
-      <c r="M14" s="61">
-        <v>0</v>
-      </c>
-      <c r="N14" s="61">
-        <v>0</v>
-      </c>
-      <c r="O14" s="61">
-        <v>0</v>
-      </c>
-      <c r="P14" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="61">
-        <v>0</v>
-      </c>
-      <c r="R14" s="61">
+      <c r="H14" s="60">
+        <v>0</v>
+      </c>
+      <c r="I14" s="60">
+        <v>0</v>
+      </c>
+      <c r="J14" s="60">
+        <v>0</v>
+      </c>
+      <c r="K14" s="60">
+        <v>0</v>
+      </c>
+      <c r="L14" s="60">
+        <v>0</v>
+      </c>
+      <c r="M14" s="60">
+        <v>0</v>
+      </c>
+      <c r="N14" s="60">
+        <v>0</v>
+      </c>
+      <c r="O14" s="60">
+        <v>0</v>
+      </c>
+      <c r="P14" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="60">
+        <v>0</v>
+      </c>
+      <c r="R14" s="60">
         <v>200</v>
       </c>
-      <c r="S14" s="61">
+      <c r="S14" s="60">
         <v>0</v>
       </c>
       <c r="T14"/>
@@ -16253,57 +16250,57 @@
       <c r="AMK14"/>
     </row>
     <row r="15" ht="14.5" spans="1:1025">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="56" t="s">
+      <c r="B15" s="65"/>
+      <c r="C15" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="61">
-        <v>0</v>
-      </c>
-      <c r="G15" s="61">
-        <v>0</v>
-      </c>
-      <c r="H15" s="61">
-        <v>0</v>
-      </c>
-      <c r="I15" s="61">
-        <v>0</v>
-      </c>
-      <c r="J15" s="61">
-        <v>0</v>
-      </c>
-      <c r="K15" s="61">
-        <v>0</v>
-      </c>
-      <c r="L15" s="61">
-        <v>0</v>
-      </c>
-      <c r="M15" s="61">
-        <v>0</v>
-      </c>
-      <c r="N15" s="61">
-        <v>0</v>
-      </c>
-      <c r="O15" s="61">
-        <v>0</v>
-      </c>
-      <c r="P15" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="61">
-        <v>0</v>
-      </c>
-      <c r="R15" s="61">
-        <v>0</v>
-      </c>
-      <c r="S15" s="61">
+      <c r="F15" s="60">
+        <v>0</v>
+      </c>
+      <c r="G15" s="60">
+        <v>0</v>
+      </c>
+      <c r="H15" s="60">
+        <v>0</v>
+      </c>
+      <c r="I15" s="60">
+        <v>0</v>
+      </c>
+      <c r="J15" s="60">
+        <v>0</v>
+      </c>
+      <c r="K15" s="60">
+        <v>0</v>
+      </c>
+      <c r="L15" s="60">
+        <v>0</v>
+      </c>
+      <c r="M15" s="60">
+        <v>0</v>
+      </c>
+      <c r="N15" s="60">
+        <v>0</v>
+      </c>
+      <c r="O15" s="60">
+        <v>0</v>
+      </c>
+      <c r="P15" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="60">
+        <v>0</v>
+      </c>
+      <c r="R15" s="60">
+        <v>0</v>
+      </c>
+      <c r="S15" s="60">
         <v>0</v>
       </c>
       <c r="T15"/>
@@ -17313,57 +17310,57 @@
       <c r="AMK15"/>
     </row>
     <row r="16" ht="14.5" spans="1:1025">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="56" t="s">
+      <c r="B16" s="63"/>
+      <c r="C16" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="60">
+      <c r="D16" s="59">
         <f t="shared" si="0"/>
         <v>747</v>
       </c>
-      <c r="F16" s="61">
-        <v>0</v>
-      </c>
-      <c r="G16" s="61">
+      <c r="F16" s="60">
+        <v>0</v>
+      </c>
+      <c r="G16" s="60">
         <v>6</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="60">
         <v>191</v>
       </c>
-      <c r="I16" s="61">
-        <v>0</v>
-      </c>
-      <c r="J16" s="61">
+      <c r="I16" s="60">
+        <v>0</v>
+      </c>
+      <c r="J16" s="60">
         <v>92</v>
       </c>
-      <c r="K16" s="61">
-        <v>0</v>
-      </c>
-      <c r="L16" s="61">
-        <v>0</v>
-      </c>
-      <c r="M16" s="61">
+      <c r="K16" s="60">
+        <v>0</v>
+      </c>
+      <c r="L16" s="60">
+        <v>0</v>
+      </c>
+      <c r="M16" s="60">
         <v>128</v>
       </c>
-      <c r="N16" s="61">
+      <c r="N16" s="60">
         <v>326</v>
       </c>
-      <c r="O16" s="61">
-        <v>0</v>
-      </c>
-      <c r="P16" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="61">
-        <v>0</v>
-      </c>
-      <c r="R16" s="61">
+      <c r="O16" s="60">
+        <v>0</v>
+      </c>
+      <c r="P16" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="60">
+        <v>0</v>
+      </c>
+      <c r="R16" s="60">
         <v>4</v>
       </c>
-      <c r="S16" s="61">
+      <c r="S16" s="60">
         <v>0</v>
       </c>
       <c r="T16"/>
@@ -18373,57 +18370,57 @@
       <c r="AMK16"/>
     </row>
     <row r="17" ht="14.5" spans="1:1025">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="56" t="s">
+      <c r="B17" s="65"/>
+      <c r="C17" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="60">
+      <c r="D17" s="59">
         <f t="shared" si="0"/>
         <v>264</v>
       </c>
-      <c r="F17" s="61">
+      <c r="F17" s="60">
         <v>8</v>
       </c>
-      <c r="G17" s="61">
-        <v>0</v>
-      </c>
-      <c r="H17" s="61">
-        <v>0</v>
-      </c>
-      <c r="I17" s="61">
-        <v>0</v>
-      </c>
-      <c r="J17" s="61">
-        <v>0</v>
-      </c>
-      <c r="K17" s="61">
-        <v>0</v>
-      </c>
-      <c r="L17" s="61">
+      <c r="G17" s="60">
+        <v>0</v>
+      </c>
+      <c r="H17" s="60">
+        <v>0</v>
+      </c>
+      <c r="I17" s="60">
+        <v>0</v>
+      </c>
+      <c r="J17" s="60">
+        <v>0</v>
+      </c>
+      <c r="K17" s="60">
+        <v>0</v>
+      </c>
+      <c r="L17" s="60">
         <v>118</v>
       </c>
-      <c r="M17" s="61">
-        <v>0</v>
-      </c>
-      <c r="N17" s="61">
+      <c r="M17" s="60">
+        <v>0</v>
+      </c>
+      <c r="N17" s="60">
         <v>138</v>
       </c>
-      <c r="O17" s="61">
-        <v>0</v>
-      </c>
-      <c r="P17" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="61">
-        <v>0</v>
-      </c>
-      <c r="R17" s="61">
-        <v>0</v>
-      </c>
-      <c r="S17" s="61">
+      <c r="O17" s="60">
+        <v>0</v>
+      </c>
+      <c r="P17" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="60">
+        <v>0</v>
+      </c>
+      <c r="R17" s="60">
+        <v>0</v>
+      </c>
+      <c r="S17" s="60">
         <v>0</v>
       </c>
       <c r="T17"/>
@@ -19433,57 +19430,57 @@
       <c r="AMK17"/>
     </row>
     <row r="18" ht="14.5" spans="1:1025">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="59">
         <f t="shared" si="0"/>
         <v>4615</v>
       </c>
-      <c r="E18" s="64"/>
-      <c r="F18" s="61">
+      <c r="E18" s="63"/>
+      <c r="F18" s="60">
         <v>1593</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="60">
         <v>1</v>
       </c>
-      <c r="H18" s="61">
+      <c r="H18" s="60">
         <v>123</v>
       </c>
-      <c r="I18" s="61">
-        <v>0</v>
-      </c>
-      <c r="J18" s="61">
+      <c r="I18" s="60">
+        <v>0</v>
+      </c>
+      <c r="J18" s="60">
         <v>1330</v>
       </c>
-      <c r="K18" s="61">
-        <v>0</v>
-      </c>
-      <c r="L18" s="61">
-        <v>0</v>
-      </c>
-      <c r="M18" s="61">
-        <v>0</v>
-      </c>
-      <c r="N18" s="61">
+      <c r="K18" s="60">
+        <v>0</v>
+      </c>
+      <c r="L18" s="60">
+        <v>0</v>
+      </c>
+      <c r="M18" s="60">
+        <v>0</v>
+      </c>
+      <c r="N18" s="60">
         <v>1563</v>
       </c>
-      <c r="O18" s="61">
+      <c r="O18" s="60">
         <v>5</v>
       </c>
-      <c r="P18" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="61">
-        <v>0</v>
-      </c>
-      <c r="R18" s="61">
-        <v>0</v>
-      </c>
-      <c r="S18" s="61">
+      <c r="P18" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="60">
+        <v>0</v>
+      </c>
+      <c r="R18" s="60">
+        <v>0</v>
+      </c>
+      <c r="S18" s="60">
         <v>0</v>
       </c>
       <c r="T18"/>
@@ -20493,57 +20490,57 @@
       <c r="AMK18"/>
     </row>
     <row r="19" ht="14.5" spans="1:1025">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="60">
+      <c r="D19" s="59">
         <f t="shared" si="0"/>
         <v>1524</v>
       </c>
-      <c r="E19" s="64"/>
-      <c r="F19" s="61">
-        <v>0</v>
-      </c>
-      <c r="G19" s="61">
+      <c r="E19" s="63"/>
+      <c r="F19" s="60">
+        <v>0</v>
+      </c>
+      <c r="G19" s="60">
         <v>456</v>
       </c>
-      <c r="H19" s="61">
-        <v>0</v>
-      </c>
-      <c r="I19" s="61">
-        <v>0</v>
-      </c>
-      <c r="J19" s="61">
-        <v>0</v>
-      </c>
-      <c r="K19" s="61">
-        <v>0</v>
-      </c>
-      <c r="L19" s="61">
-        <v>0</v>
-      </c>
-      <c r="M19" s="61">
-        <v>0</v>
-      </c>
-      <c r="N19" s="61">
-        <v>0</v>
-      </c>
-      <c r="O19" s="61">
+      <c r="H19" s="60">
+        <v>0</v>
+      </c>
+      <c r="I19" s="60">
+        <v>0</v>
+      </c>
+      <c r="J19" s="60">
+        <v>0</v>
+      </c>
+      <c r="K19" s="60">
+        <v>0</v>
+      </c>
+      <c r="L19" s="60">
+        <v>0</v>
+      </c>
+      <c r="M19" s="60">
+        <v>0</v>
+      </c>
+      <c r="N19" s="60">
+        <v>0</v>
+      </c>
+      <c r="O19" s="60">
         <v>493</v>
       </c>
-      <c r="P19" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="61">
-        <v>0</v>
-      </c>
-      <c r="R19" s="61">
-        <v>0</v>
-      </c>
-      <c r="S19" s="61">
+      <c r="P19" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="60">
+        <v>0</v>
+      </c>
+      <c r="R19" s="60">
+        <v>0</v>
+      </c>
+      <c r="S19" s="60">
         <v>575</v>
       </c>
       <c r="T19"/>
@@ -21553,57 +21550,57 @@
       <c r="AMK19"/>
     </row>
     <row r="20" ht="14.5" spans="1:1025">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="59">
         <f t="shared" si="0"/>
         <v>530</v>
       </c>
-      <c r="E20" s="64"/>
-      <c r="F20" s="61">
-        <v>0</v>
-      </c>
-      <c r="G20" s="61">
+      <c r="E20" s="63"/>
+      <c r="F20" s="60">
+        <v>0</v>
+      </c>
+      <c r="G20" s="60">
         <v>7</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="60">
         <v>146</v>
       </c>
-      <c r="I20" s="61">
-        <v>0</v>
-      </c>
-      <c r="J20" s="61">
-        <v>0</v>
-      </c>
-      <c r="K20" s="61">
-        <v>0</v>
-      </c>
-      <c r="L20" s="61">
-        <v>0</v>
-      </c>
-      <c r="M20" s="61">
-        <v>0</v>
-      </c>
-      <c r="N20" s="61">
-        <v>0</v>
-      </c>
-      <c r="O20" s="61">
+      <c r="I20" s="60">
+        <v>0</v>
+      </c>
+      <c r="J20" s="60">
+        <v>0</v>
+      </c>
+      <c r="K20" s="60">
+        <v>0</v>
+      </c>
+      <c r="L20" s="60">
+        <v>0</v>
+      </c>
+      <c r="M20" s="60">
+        <v>0</v>
+      </c>
+      <c r="N20" s="60">
+        <v>0</v>
+      </c>
+      <c r="O20" s="60">
         <v>1</v>
       </c>
-      <c r="P20" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="61">
-        <v>0</v>
-      </c>
-      <c r="R20" s="61">
-        <v>0</v>
-      </c>
-      <c r="S20" s="61">
+      <c r="P20" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="60">
+        <v>0</v>
+      </c>
+      <c r="R20" s="60">
+        <v>0</v>
+      </c>
+      <c r="S20" s="60">
         <v>376</v>
       </c>
       <c r="T20"/>
@@ -22613,9 +22610,9 @@
       <c r="AMK20"/>
     </row>
     <row r="21" spans="1:1025">
-      <c r="A21" s="60"/>
+      <c r="A21" s="59"/>
       <c r="C21"/>
-      <c r="D21" s="60"/>
+      <c r="D21" s="59"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
@@ -23637,40 +23634,40 @@
       <c r="AMJ21"/>
       <c r="AMK21"/>
     </row>
-    <row r="22" s="57" customFormat="1" spans="1:18">
-      <c r="A22" s="67" t="s">
+    <row r="22" s="56" customFormat="1" spans="1:18">
+      <c r="A22" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="D22" s="61">
+      <c r="B22" s="60"/>
+      <c r="D22" s="60">
         <f>SUM(F22:S22)</f>
         <v>47</v>
       </c>
-      <c r="F22" s="57">
+      <c r="F22" s="56">
         <v>11</v>
       </c>
-      <c r="G22" s="57">
+      <c r="G22" s="56">
         <v>2</v>
       </c>
-      <c r="H22" s="57">
+      <c r="H22" s="56">
         <v>1</v>
       </c>
-      <c r="K22" s="57">
+      <c r="K22" s="56">
         <v>5</v>
       </c>
-      <c r="L22" s="57">
+      <c r="L22" s="56">
         <v>3</v>
       </c>
-      <c r="M22" s="57">
+      <c r="M22" s="56">
         <v>3</v>
       </c>
-      <c r="O22" s="57">
+      <c r="O22" s="56">
         <v>19</v>
       </c>
-      <c r="Q22" s="57">
+      <c r="Q22" s="56">
         <v>1</v>
       </c>
-      <c r="R22" s="57">
+      <c r="R22" s="56">
         <v>2</v>
       </c>
     </row>
@@ -23687,122 +23684,122 @@
       <c r="AMJ23"/>
       <c r="AMK23"/>
     </row>
-    <row r="24" s="60" customFormat="1" spans="1:19">
-      <c r="A24" s="60" t="s">
+    <row r="24" s="59" customFormat="1" spans="1:19">
+      <c r="A24" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="D24" s="60">
+      <c r="B24" s="60"/>
+      <c r="D24" s="59">
         <f>SUM(F24:S24)</f>
         <v>52098</v>
       </c>
-      <c r="F24" s="60">
+      <c r="F24" s="59">
         <f t="shared" ref="F24:S24" si="1">SUM(F2:F22)</f>
         <v>5544</v>
       </c>
-      <c r="G24" s="60">
+      <c r="G24" s="59">
         <f t="shared" si="1"/>
         <v>2405</v>
       </c>
-      <c r="H24" s="60">
+      <c r="H24" s="59">
         <f t="shared" si="1"/>
         <v>11253</v>
       </c>
-      <c r="I24" s="60">
+      <c r="I24" s="59">
         <f t="shared" si="1"/>
         <v>2488</v>
       </c>
-      <c r="J24" s="60">
+      <c r="J24" s="59">
         <f t="shared" si="1"/>
         <v>4567</v>
       </c>
-      <c r="K24" s="60">
+      <c r="K24" s="59">
         <f t="shared" si="1"/>
         <v>4445</v>
       </c>
-      <c r="L24" s="60">
+      <c r="L24" s="59">
         <f t="shared" si="1"/>
         <v>3556</v>
       </c>
-      <c r="M24" s="60">
+      <c r="M24" s="59">
         <f t="shared" si="1"/>
         <v>1768</v>
       </c>
-      <c r="N24" s="60">
+      <c r="N24" s="59">
         <f t="shared" si="1"/>
         <v>3515</v>
       </c>
-      <c r="O24" s="60">
+      <c r="O24" s="59">
         <f t="shared" si="1"/>
         <v>4993</v>
       </c>
-      <c r="P24" s="60">
+      <c r="P24" s="59">
         <f t="shared" si="1"/>
         <v>2204</v>
       </c>
-      <c r="Q24" s="60">
+      <c r="Q24" s="59">
         <f t="shared" si="1"/>
         <v>2093</v>
       </c>
-      <c r="R24" s="60">
+      <c r="R24" s="59">
         <f t="shared" si="1"/>
         <v>1721</v>
       </c>
-      <c r="S24" s="60">
+      <c r="S24" s="59">
         <f t="shared" si="1"/>
         <v>1546</v>
       </c>
     </row>
     <row r="25" spans="1:1025">
-      <c r="A25" s="67" t="s">
+      <c r="A25" s="66" t="s">
         <v>59</v>
       </c>
       <c r="C25"/>
-      <c r="D25" s="61">
+      <c r="D25" s="60">
         <f>SUM(F25:S25)</f>
         <v>1238</v>
       </c>
       <c r="E25"/>
-      <c r="F25" s="61">
+      <c r="F25" s="60">
         <v>143</v>
       </c>
-      <c r="G25" s="61">
+      <c r="G25" s="60">
         <v>93</v>
       </c>
-      <c r="H25" s="61">
+      <c r="H25" s="60">
         <v>114</v>
       </c>
-      <c r="I25" s="61">
+      <c r="I25" s="60">
         <v>23</v>
       </c>
-      <c r="J25" s="61">
+      <c r="J25" s="60">
         <v>148</v>
       </c>
-      <c r="K25" s="61">
+      <c r="K25" s="60">
         <v>43</v>
       </c>
-      <c r="L25" s="61">
+      <c r="L25" s="60">
         <v>83</v>
       </c>
-      <c r="M25" s="61">
+      <c r="M25" s="60">
         <v>94</v>
       </c>
-      <c r="N25" s="61">
+      <c r="N25" s="60">
         <v>132</v>
       </c>
-      <c r="O25" s="61">
+      <c r="O25" s="60">
         <v>143</v>
       </c>
-      <c r="P25" s="61">
+      <c r="P25" s="60">
         <v>76</v>
       </c>
-      <c r="Q25" s="61">
+      <c r="Q25" s="60">
         <v>30</v>
       </c>
-      <c r="R25" s="61">
+      <c r="R25" s="60">
         <v>94</v>
       </c>
-      <c r="S25" s="61">
+      <c r="S25" s="60">
         <v>22</v>
       </c>
       <c r="AME25"/>
@@ -23815,7 +23812,7 @@
     </row>
     <row r="26" spans="3:23">
       <c r="C26"/>
-      <c r="D26" s="60"/>
+      <c r="D26" s="59"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
@@ -23881,102 +23878,102 @@
     </row>
     <row r="29" spans="3:24">
       <c r="C29"/>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="60" t="s">
+      <c r="E29" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="63" t="s">
+      <c r="F29" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="63" t="s">
+      <c r="G29" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="63" t="s">
+      <c r="H29" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="63" t="s">
+      <c r="I29" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="J29" s="63" t="s">
+      <c r="J29" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="K29" s="63" t="s">
+      <c r="K29" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L29" s="63" t="s">
+      <c r="L29" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="M29" s="63" t="s">
+      <c r="M29" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="N29" s="63" t="s">
+      <c r="N29" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="O29" s="63" t="s">
+      <c r="O29" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="P29" s="63" t="s">
+      <c r="P29" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="Q29" s="63" t="s">
+      <c r="Q29" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="R29" s="63" t="s">
+      <c r="R29" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="S29" s="63" t="s">
+      <c r="S29" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="U29" s="63" t="s">
+      <c r="U29" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="V29" s="63" t="s">
+      <c r="V29" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="W29" s="63" t="s">
+      <c r="W29" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="X29" s="61" t="s">
+      <c r="X29" s="60" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="3:23">
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="68" t="s">
+      <c r="D30" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="61">
+      <c r="E30" s="60">
         <f>SUM(F30,J30,N30,P30,S30)</f>
         <v>85</v>
       </c>
-      <c r="F30" s="61">
+      <c r="F30" s="60">
         <v>44</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30" s="61">
+      <c r="J30" s="60">
         <v>12</v>
       </c>
       <c r="K30"/>
       <c r="L30"/>
-      <c r="M30" s="67" t="s">
+      <c r="M30" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="N30" s="61">
+      <c r="N30" s="60">
         <v>7</v>
       </c>
       <c r="O30"/>
-      <c r="P30" s="61">
+      <c r="P30" s="60">
         <v>19</v>
       </c>
       <c r="Q30"/>
       <c r="R30"/>
-      <c r="S30" s="61">
+      <c r="S30" s="60">
         <v>3</v>
       </c>
       <c r="V30"/>
@@ -23984,50 +23981,50 @@
     </row>
     <row r="31" spans="3:23">
       <c r="C31"/>
-      <c r="D31" s="68" t="s">
+      <c r="D31" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="61">
+      <c r="E31" s="60">
         <f>SUM(F31,J31,N31,P31,S31)</f>
         <v>3329</v>
       </c>
-      <c r="F31" s="61">
+      <c r="F31" s="60">
         <v>1554</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
-      <c r="J31" s="61">
+      <c r="J31" s="60">
         <v>538</v>
       </c>
       <c r="K31"/>
       <c r="L31"/>
-      <c r="M31" s="67" t="s">
+      <c r="M31" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="N31" s="61">
+      <c r="N31" s="60">
         <v>111</v>
       </c>
       <c r="O31"/>
-      <c r="P31" s="61">
+      <c r="P31" s="60">
         <v>623</v>
       </c>
       <c r="Q31"/>
       <c r="R31"/>
-      <c r="S31" s="61">
+      <c r="S31" s="60">
         <v>503</v>
       </c>
       <c r="V31"/>
       <c r="W31"/>
     </row>
     <row r="32" spans="3:23">
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="68" t="s">
+      <c r="D32" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="61">
+      <c r="E32" s="60">
         <f>SUM(O32,P32,Q32,S32)</f>
         <v>55</v>
       </c>
@@ -24038,21 +24035,21 @@
       <c r="J32"/>
       <c r="K32"/>
       <c r="L32"/>
-      <c r="M32" s="67" t="s">
+      <c r="M32" s="66" t="s">
         <v>63</v>
       </c>
       <c r="N32"/>
-      <c r="O32" s="61">
+      <c r="O32" s="60">
         <v>23</v>
       </c>
-      <c r="P32" s="61">
+      <c r="P32" s="60">
         <v>13</v>
       </c>
-      <c r="Q32" s="61">
+      <c r="Q32" s="60">
         <v>15</v>
       </c>
       <c r="R32"/>
-      <c r="S32" s="61">
+      <c r="S32" s="60">
         <v>4</v>
       </c>
       <c r="V32"/>
@@ -24060,10 +24057,10 @@
     </row>
     <row r="33" spans="3:23">
       <c r="C33"/>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="61">
+      <c r="E33" s="60">
         <f>SUM(O33,P33,Q33,S33)</f>
         <v>1739</v>
       </c>
@@ -24074,63 +24071,63 @@
       <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
-      <c r="M33" s="61">
+      <c r="M33" s="60">
         <v>100</v>
       </c>
       <c r="N33"/>
-      <c r="O33" s="61">
+      <c r="O33" s="60">
         <v>958</v>
       </c>
-      <c r="P33" s="61">
+      <c r="P33" s="60">
         <v>200</v>
       </c>
-      <c r="Q33" s="61">
+      <c r="Q33" s="60">
         <v>211</v>
       </c>
       <c r="R33"/>
-      <c r="S33" s="61">
+      <c r="S33" s="60">
         <v>370</v>
       </c>
       <c r="V33"/>
       <c r="W33"/>
     </row>
     <row r="34" spans="3:23">
-      <c r="C34" s="61" t="s">
+      <c r="C34" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="61">
+      <c r="E34" s="60">
         <f t="shared" ref="E34:E59" si="2">SUM(F34:S34)</f>
         <v>73</v>
       </c>
       <c r="F34"/>
-      <c r="G34" s="61">
+      <c r="G34" s="60">
         <v>16</v>
       </c>
-      <c r="H34" s="61">
+      <c r="H34" s="60">
         <v>15</v>
       </c>
-      <c r="I34" s="61">
+      <c r="I34" s="60">
         <v>7</v>
       </c>
-      <c r="J34" s="61">
+      <c r="J34" s="60">
         <v>17</v>
       </c>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
-      <c r="N34" s="61">
+      <c r="N34" s="60">
         <v>4</v>
       </c>
       <c r="O34"/>
       <c r="P34"/>
-      <c r="Q34" s="61">
+      <c r="Q34" s="60">
         <v>12</v>
       </c>
       <c r="R34"/>
-      <c r="S34" s="61">
+      <c r="S34" s="60">
         <v>2</v>
       </c>
       <c r="V34"/>
@@ -24138,54 +24135,54 @@
     </row>
     <row r="35" spans="3:23">
       <c r="C35"/>
-      <c r="D35" s="68" t="s">
+      <c r="D35" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="61">
+      <c r="E35" s="60">
         <f t="shared" si="2"/>
         <v>5277</v>
       </c>
       <c r="F35"/>
-      <c r="G35" s="61">
+      <c r="G35" s="60">
         <v>424</v>
       </c>
-      <c r="H35" s="61">
+      <c r="H35" s="60">
         <v>3339</v>
       </c>
-      <c r="I35" s="61">
+      <c r="I35" s="60">
         <v>667</v>
       </c>
-      <c r="J35" s="61">
+      <c r="J35" s="60">
         <v>383</v>
       </c>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
-      <c r="N35" s="61">
+      <c r="N35" s="60">
         <v>136</v>
       </c>
       <c r="O35"/>
       <c r="P35"/>
-      <c r="Q35" s="61">
+      <c r="Q35" s="60">
         <v>45</v>
       </c>
       <c r="R35"/>
-      <c r="S35" s="61">
+      <c r="S35" s="60">
         <v>283</v>
       </c>
       <c r="V35"/>
-      <c r="W35" s="61">
+      <c r="W35" s="60">
         <v>1912</v>
       </c>
     </row>
     <row r="36" spans="3:23">
-      <c r="C36" s="61" t="s">
+      <c r="C36" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="63" t="s">
+      <c r="D36" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="61">
+      <c r="E36" s="60">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -24194,7 +24191,7 @@
       <c r="H36"/>
       <c r="J36"/>
       <c r="K36"/>
-      <c r="L36" s="61">
+      <c r="L36" s="60">
         <v>10</v>
       </c>
       <c r="M36"/>
@@ -24209,10 +24206,10 @@
     </row>
     <row r="37" spans="3:23">
       <c r="C37"/>
-      <c r="D37" s="63" t="s">
+      <c r="D37" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="61">
+      <c r="E37" s="60">
         <f t="shared" si="2"/>
         <v>248</v>
       </c>
@@ -24221,7 +24218,7 @@
       <c r="H37"/>
       <c r="J37"/>
       <c r="K37"/>
-      <c r="L37" s="61">
+      <c r="L37" s="60">
         <v>248</v>
       </c>
       <c r="M37"/>
@@ -24232,18 +24229,18 @@
       <c r="R37"/>
       <c r="S37"/>
       <c r="V37"/>
-      <c r="W37" s="61">
+      <c r="W37" s="60">
         <v>8000</v>
       </c>
     </row>
     <row r="38" spans="3:23">
-      <c r="C38" s="61" t="s">
+      <c r="C38" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="61">
+      <c r="E38" s="60">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -24257,10 +24254,10 @@
       <c r="N38"/>
       <c r="O38"/>
       <c r="P38"/>
-      <c r="Q38" s="61">
+      <c r="Q38" s="60">
         <v>1</v>
       </c>
-      <c r="R38" s="61">
+      <c r="R38" s="60">
         <v>44</v>
       </c>
       <c r="S38"/>
@@ -24269,10 +24266,10 @@
     </row>
     <row r="39" spans="3:23">
       <c r="C39"/>
-      <c r="D39" s="68" t="s">
+      <c r="D39" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="61">
+      <c r="E39" s="60">
         <f t="shared" si="2"/>
         <v>1258</v>
       </c>
@@ -24286,56 +24283,56 @@
       <c r="N39"/>
       <c r="O39"/>
       <c r="P39"/>
-      <c r="Q39" s="61">
+      <c r="Q39" s="60">
         <v>701</v>
       </c>
-      <c r="R39" s="61">
+      <c r="R39" s="60">
         <v>557</v>
       </c>
       <c r="S39"/>
-      <c r="V39" s="61">
+      <c r="V39" s="60">
         <v>2000</v>
       </c>
       <c r="W39"/>
     </row>
     <row r="40" spans="3:23">
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="68" t="s">
+      <c r="D40" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="61">
+      <c r="E40" s="60">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
       <c r="H40"/>
-      <c r="J40" s="61">
+      <c r="J40" s="60">
         <v>15</v>
       </c>
-      <c r="K40" s="61">
+      <c r="K40" s="60">
         <v>12</v>
       </c>
       <c r="L40"/>
-      <c r="M40" s="61">
+      <c r="M40" s="60">
         <v>24</v>
       </c>
-      <c r="N40" s="61">
+      <c r="N40" s="60">
         <v>9</v>
       </c>
-      <c r="O40" s="61">
+      <c r="O40" s="60">
         <v>17</v>
       </c>
-      <c r="P40" s="61">
+      <c r="P40" s="60">
         <v>13</v>
       </c>
-      <c r="Q40" s="61">
+      <c r="Q40" s="60">
         <v>1</v>
       </c>
       <c r="R40"/>
-      <c r="S40" s="61">
+      <c r="S40" s="60">
         <v>8</v>
       </c>
       <c r="V40"/>
@@ -24343,57 +24340,57 @@
     </row>
     <row r="41" spans="3:23">
       <c r="C41"/>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="61">
+      <c r="E41" s="60">
         <f t="shared" si="2"/>
         <v>4002</v>
       </c>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
-      <c r="J41" s="61">
+      <c r="J41" s="60">
         <v>335</v>
       </c>
-      <c r="K41" s="61">
+      <c r="K41" s="60">
         <v>880</v>
       </c>
       <c r="L41"/>
-      <c r="M41" s="61">
+      <c r="M41" s="60">
         <v>403</v>
       </c>
-      <c r="N41" s="61">
+      <c r="N41" s="60">
         <v>174</v>
       </c>
-      <c r="O41" s="61">
+      <c r="O41" s="60">
         <v>937</v>
       </c>
-      <c r="P41" s="61">
+      <c r="P41" s="60">
         <v>325</v>
       </c>
-      <c r="Q41" s="61">
+      <c r="Q41" s="60">
         <v>635</v>
       </c>
       <c r="R41"/>
-      <c r="S41" s="61">
+      <c r="S41" s="60">
         <v>313</v>
       </c>
       <c r="V41"/>
       <c r="W41"/>
     </row>
     <row r="42" spans="3:23">
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="68" t="s">
+      <c r="D42" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="61">
+      <c r="E42" s="60">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="F42" s="61">
+      <c r="F42" s="60">
         <v>27</v>
       </c>
       <c r="G42"/>
@@ -24405,11 +24402,11 @@
       <c r="N42"/>
       <c r="O42"/>
       <c r="P42"/>
-      <c r="Q42" s="61">
+      <c r="Q42" s="60">
         <v>1</v>
       </c>
       <c r="R42"/>
-      <c r="S42" s="61">
+      <c r="S42" s="60">
         <v>5</v>
       </c>
       <c r="V42"/>
@@ -24417,14 +24414,14 @@
     </row>
     <row r="43" spans="3:23">
       <c r="C43"/>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="61">
+      <c r="E43" s="60">
         <f t="shared" si="2"/>
         <v>1650</v>
       </c>
-      <c r="F43" s="61">
+      <c r="F43" s="60">
         <v>1072</v>
       </c>
       <c r="G43"/>
@@ -24436,26 +24433,26 @@
       <c r="N43"/>
       <c r="O43"/>
       <c r="P43"/>
-      <c r="Q43" s="61">
+      <c r="Q43" s="60">
         <v>501</v>
       </c>
       <c r="R43"/>
-      <c r="S43" s="61">
+      <c r="S43" s="60">
         <v>77</v>
       </c>
       <c r="V43"/>
-      <c r="W43" s="61">
+      <c r="W43" s="60">
         <v>900</v>
       </c>
     </row>
     <row r="44" spans="3:23">
-      <c r="C44" s="61" t="s">
+      <c r="C44" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="68" t="s">
+      <c r="D44" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="61">
+      <c r="E44" s="60">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -24465,14 +24462,14 @@
       <c r="K44"/>
       <c r="L44"/>
       <c r="M44"/>
-      <c r="N44" s="61">
+      <c r="N44" s="60">
         <v>16</v>
       </c>
-      <c r="O44" s="61">
+      <c r="O44" s="60">
         <v>12</v>
       </c>
       <c r="P44"/>
-      <c r="R44" s="61">
+      <c r="R44" s="60">
         <v>7</v>
       </c>
       <c r="V44"/>
@@ -24480,10 +24477,10 @@
     </row>
     <row r="45" spans="3:23">
       <c r="C45"/>
-      <c r="D45" s="68" t="s">
+      <c r="D45" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="61">
+      <c r="E45" s="60">
         <f t="shared" si="2"/>
         <v>1223</v>
       </c>
@@ -24493,39 +24490,39 @@
       <c r="K45"/>
       <c r="L45"/>
       <c r="M45"/>
-      <c r="N45" s="61">
+      <c r="N45" s="60">
         <v>428</v>
       </c>
-      <c r="O45" s="61">
+      <c r="O45" s="60">
         <v>759</v>
       </c>
       <c r="P45"/>
-      <c r="R45" s="61">
+      <c r="R45" s="60">
         <v>36</v>
       </c>
       <c r="V45"/>
-      <c r="W45" s="61">
+      <c r="W45" s="60">
         <v>7000</v>
       </c>
     </row>
     <row r="46" spans="3:23">
-      <c r="C46" s="61" t="s">
+      <c r="C46" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="68" t="s">
+      <c r="D46" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="61">
+      <c r="E46" s="60">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="G46" s="61">
+      <c r="G46" s="60">
         <v>8</v>
       </c>
-      <c r="H46" s="61">
+      <c r="H46" s="60">
         <v>12</v>
       </c>
-      <c r="J46" s="61">
+      <c r="J46" s="60">
         <v>26</v>
       </c>
       <c r="K46"/>
@@ -24534,7 +24531,7 @@
       <c r="N46"/>
       <c r="O46"/>
       <c r="P46"/>
-      <c r="R46" s="61">
+      <c r="R46" s="60">
         <v>6</v>
       </c>
       <c r="V46"/>
@@ -24542,20 +24539,20 @@
     </row>
     <row r="47" spans="3:23">
       <c r="C47"/>
-      <c r="D47" s="68" t="s">
+      <c r="D47" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="61">
+      <c r="E47" s="60">
         <f t="shared" si="2"/>
         <v>3780</v>
       </c>
-      <c r="G47" s="61">
+      <c r="G47" s="60">
         <v>507</v>
       </c>
-      <c r="H47" s="61">
+      <c r="H47" s="60">
         <v>2950</v>
       </c>
-      <c r="J47" s="61">
+      <c r="J47" s="60">
         <v>303</v>
       </c>
       <c r="K47"/>
@@ -24564,36 +24561,36 @@
       <c r="N47"/>
       <c r="O47"/>
       <c r="P47"/>
-      <c r="R47" s="61">
+      <c r="R47" s="60">
         <v>20</v>
       </c>
       <c r="V47"/>
-      <c r="W47" s="61">
+      <c r="W47" s="60">
         <v>2800</v>
       </c>
     </row>
     <row r="48" spans="3:23">
-      <c r="C48" s="61" t="s">
+      <c r="C48" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="68" t="s">
+      <c r="D48" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="61">
+      <c r="E48" s="60">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="J48"/>
-      <c r="K48" s="61">
+      <c r="K48" s="60">
         <v>8</v>
       </c>
-      <c r="L48" s="61">
+      <c r="L48" s="60">
         <v>16</v>
       </c>
       <c r="M48"/>
       <c r="N48"/>
       <c r="O48"/>
-      <c r="P48" s="61">
+      <c r="P48" s="60">
         <v>31</v>
       </c>
       <c r="R48"/>
@@ -24602,42 +24599,42 @@
     </row>
     <row r="49" spans="3:23">
       <c r="C49"/>
-      <c r="D49" s="68" t="s">
+      <c r="D49" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E49" s="61">
+      <c r="E49" s="60">
         <f t="shared" si="2"/>
         <v>2684</v>
       </c>
       <c r="J49"/>
-      <c r="K49" s="61">
+      <c r="K49" s="60">
         <v>1192</v>
       </c>
-      <c r="L49" s="61">
+      <c r="L49" s="60">
         <v>436</v>
       </c>
       <c r="M49"/>
       <c r="N49"/>
       <c r="O49"/>
-      <c r="P49" s="61">
+      <c r="P49" s="60">
         <v>1056</v>
       </c>
       <c r="R49"/>
-      <c r="V49" s="67" t="s">
+      <c r="V49" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="W49" s="67" t="s">
+      <c r="W49" s="66" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="3:23">
-      <c r="C50" s="61" t="s">
+      <c r="C50" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="68" t="s">
+      <c r="D50" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="61">
+      <c r="E50" s="60">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -24645,24 +24642,24 @@
       <c r="K50"/>
       <c r="L50"/>
       <c r="M50"/>
-      <c r="N50" s="61">
+      <c r="N50" s="60">
         <v>20</v>
       </c>
       <c r="O50"/>
       <c r="R50"/>
-      <c r="V50" s="67" t="s">
+      <c r="V50" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="W50" s="67" t="s">
+      <c r="W50" s="66" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="51" spans="3:23">
       <c r="C51"/>
-      <c r="D51" s="68" t="s">
+      <c r="D51" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E51" s="61">
+      <c r="E51" s="60">
         <f t="shared" si="2"/>
         <v>288</v>
       </c>
@@ -24670,247 +24667,247 @@
       <c r="K51"/>
       <c r="L51"/>
       <c r="M51"/>
-      <c r="N51" s="61">
+      <c r="N51" s="60">
         <v>288</v>
       </c>
       <c r="O51"/>
       <c r="R51"/>
-      <c r="V51" s="61">
+      <c r="V51" s="60">
         <v>35000</v>
       </c>
-      <c r="W51" s="61">
+      <c r="W51" s="60">
         <v>35000</v>
       </c>
     </row>
     <row r="52" spans="3:18">
-      <c r="C52" s="61" t="s">
+      <c r="C52" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="68" t="s">
+      <c r="D52" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E52" s="61">
+      <c r="E52" s="60">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="J52"/>
-      <c r="K52" s="61">
+      <c r="K52" s="60">
         <v>8</v>
       </c>
       <c r="L52"/>
-      <c r="M52" s="61">
+      <c r="M52" s="60">
         <v>20</v>
       </c>
-      <c r="O52" s="61">
+      <c r="O52" s="60">
         <v>24</v>
       </c>
-      <c r="R52" s="61">
+      <c r="R52" s="60">
         <v>15</v>
       </c>
     </row>
     <row r="53" spans="3:18">
       <c r="C53"/>
-      <c r="D53" s="68" t="s">
+      <c r="D53" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E53" s="61">
+      <c r="E53" s="60">
         <f t="shared" si="2"/>
         <v>2373</v>
       </c>
       <c r="J53"/>
-      <c r="K53" s="61">
+      <c r="K53" s="60">
         <v>1073</v>
       </c>
       <c r="L53"/>
-      <c r="M53" s="61">
+      <c r="M53" s="60">
         <v>554</v>
       </c>
-      <c r="O53" s="61">
+      <c r="O53" s="60">
         <v>665</v>
       </c>
-      <c r="R53" s="61">
+      <c r="R53" s="60">
         <v>81</v>
       </c>
     </row>
     <row r="54" spans="3:18">
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="68" t="s">
+      <c r="D54" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="61">
+      <c r="E54" s="60">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="J54" s="61">
+      <c r="J54" s="60">
         <v>38</v>
       </c>
       <c r="L54"/>
-      <c r="R54" s="61">
+      <c r="R54" s="60">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="3:18">
       <c r="C55"/>
-      <c r="D55" s="68" t="s">
+      <c r="D55" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E55" s="61">
+      <c r="E55" s="60">
         <f t="shared" si="2"/>
         <v>1146</v>
       </c>
-      <c r="J55" s="61">
+      <c r="J55" s="60">
         <v>868</v>
       </c>
       <c r="L55"/>
-      <c r="R55" s="61">
+      <c r="R55" s="60">
         <v>278</v>
       </c>
     </row>
     <row r="56" spans="3:18">
-      <c r="C56" s="61" t="s">
+      <c r="C56" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="D56" s="68" t="s">
+      <c r="D56" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="61">
+      <c r="E56" s="60">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="L56" s="61">
+      <c r="L56" s="60">
         <v>16</v>
       </c>
       <c r="R56"/>
     </row>
     <row r="57" spans="3:18">
       <c r="C57"/>
-      <c r="D57" s="68" t="s">
+      <c r="D57" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="61">
+      <c r="E57" s="60">
         <f t="shared" si="2"/>
         <v>491</v>
       </c>
-      <c r="L57" s="61">
+      <c r="L57" s="60">
         <v>491</v>
       </c>
       <c r="R57"/>
     </row>
     <row r="58" spans="3:18">
-      <c r="C58" s="61" t="s">
+      <c r="C58" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="68" t="s">
+      <c r="D58" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="61">
+      <c r="E58" s="60">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="R58" s="61">
+      <c r="R58" s="60">
         <v>6</v>
       </c>
     </row>
     <row r="59" spans="4:18">
-      <c r="D59" s="68" t="s">
+      <c r="D59" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="61">
+      <c r="E59" s="60">
         <f t="shared" si="2"/>
         <v>189</v>
       </c>
-      <c r="R59" s="61">
+      <c r="R59" s="60">
         <v>189</v>
       </c>
     </row>
     <row r="61" spans="3:24">
-      <c r="C61" s="61" t="s">
+      <c r="C61" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="68" t="s">
+      <c r="D61" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="F61" s="61">
+      <c r="F61" s="60">
         <v>16</v>
       </c>
-      <c r="H61" s="61">
+      <c r="H61" s="60">
         <v>15</v>
       </c>
-      <c r="O61" s="61">
+      <c r="O61" s="60">
         <v>17</v>
       </c>
-      <c r="R61" s="61">
+      <c r="R61" s="60">
         <v>6</v>
       </c>
-      <c r="U61" s="61" t="s">
+      <c r="U61" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="V61" s="61">
+      <c r="V61" s="60">
         <v>10000</v>
       </c>
-      <c r="W61" s="61">
+      <c r="W61" s="60">
         <v>10000</v>
       </c>
-      <c r="X61" s="61">
+      <c r="X61" s="60">
         <v>7000</v>
       </c>
     </row>
     <row r="62" spans="4:18">
-      <c r="D62" s="68" t="s">
+      <c r="D62" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="F62" s="61">
+      <c r="F62" s="60">
         <v>1423</v>
       </c>
-      <c r="H62" s="61">
+      <c r="H62" s="60">
         <v>146</v>
       </c>
-      <c r="O62" s="61">
+      <c r="O62" s="60">
         <v>493</v>
       </c>
-      <c r="R62" s="61">
+      <c r="R62" s="60">
         <v>560</v>
       </c>
     </row>
     <row r="63" spans="3:24">
-      <c r="C63" s="61" t="s">
+      <c r="C63" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D63" s="68" t="s">
+      <c r="D63" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="J63" s="61">
+      <c r="J63" s="60">
         <v>8</v>
       </c>
-      <c r="L63" s="61">
+      <c r="L63" s="60">
         <v>9</v>
       </c>
-      <c r="M63" s="61">
+      <c r="M63" s="60">
         <v>10</v>
       </c>
-      <c r="V63" s="61">
+      <c r="V63" s="60">
         <v>40000</v>
       </c>
-      <c r="X63" s="61">
+      <c r="X63" s="60">
         <v>10000</v>
       </c>
     </row>
     <row r="64" spans="4:23">
-      <c r="D64" s="68" t="s">
+      <c r="D64" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="J64" s="61">
+      <c r="J64" s="60">
         <v>1287</v>
       </c>
-      <c r="L64" s="61">
+      <c r="L64" s="60">
         <v>118</v>
       </c>
-      <c r="M64" s="61">
+      <c r="M64" s="60">
         <v>128</v>
       </c>
-      <c r="W64" s="61">
+      <c r="W64" s="60">
         <v>4000</v>
       </c>
     </row>
@@ -24923,7 +24920,7 @@
       <c r="AMK67"/>
     </row>
     <row r="68" spans="4:1025">
-      <c r="D68" s="61"/>
+      <c r="D68" s="60"/>
       <c r="ALW68"/>
       <c r="ALX68"/>
       <c r="ALY68"/>
@@ -25176,239 +25173,239 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.1727272727273" style="53"/>
-    <col min="3" max="3" width="13.1727272727273" style="53"/>
-    <col min="4" max="4" width="26.5636363636364" style="53"/>
-    <col min="5" max="1024" width="9" style="53"/>
+    <col min="1" max="1" width="13.1727272727273" style="52"/>
+    <col min="3" max="3" width="13.1727272727273" style="52"/>
+    <col min="4" max="4" width="26.5636363636364" style="52"/>
+    <col min="5" max="1024" width="9" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="55" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="55" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="53" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="55" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="55" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="55" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="55" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="55" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="55" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="57" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="55" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="53" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="E14" s="56" t="s">
+      <c r="C14" s="56"/>
+      <c r="E14" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="53" t="s">
         <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="E15" s="56" t="s">
+      <c r="C15" s="56"/>
+      <c r="E15" s="55" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="53" t="s">
         <v>49</v>
       </c>
       <c r="B16" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="E16" s="56" t="s">
+      <c r="C16" s="56"/>
+      <c r="E16" s="55" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="53" t="s">
         <v>51</v>
       </c>
       <c r="B17" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="E17" s="56" t="s">
+      <c r="C17" s="56"/>
+      <c r="E17" s="55" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="58" t="s">
         <v>146</v>
       </c>
       <c r="B18" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="E18" s="56" t="s">
+      <c r="C18" s="56"/>
+      <c r="E18" s="55" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="53" t="s">
         <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>148</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="E19" s="56" t="s">
+      <c r="C19" s="56"/>
+      <c r="E19" s="55" t="s">
         <v>56</v>
       </c>
     </row>
@@ -25424,7 +25421,7 @@
   <sheetPr/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -25461,13 +25458,13 @@
       <c r="H1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="50" t="s">
         <v>153</v>
       </c>
     </row>
@@ -25491,7 +25488,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="49"/>
-      <c r="J2" s="52">
+      <c r="J2" s="51">
         <v>6919</v>
       </c>
       <c r="K2" s="49">
@@ -25518,7 +25515,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="49"/>
-      <c r="J3" s="52">
+      <c r="J3" s="51">
         <v>4201</v>
       </c>
       <c r="K3" s="49">
@@ -25545,7 +25542,7 @@
         <v>27</v>
       </c>
       <c r="I4" s="49"/>
-      <c r="J4" s="52">
+      <c r="J4" s="51">
         <v>425</v>
       </c>
       <c r="K4" s="49">
@@ -25572,7 +25569,7 @@
         <v>35</v>
       </c>
       <c r="I5" s="49"/>
-      <c r="J5" s="52">
+      <c r="J5" s="51">
         <v>2377</v>
       </c>
       <c r="K5" s="49">
@@ -25601,7 +25598,7 @@
       <c r="I6" s="49">
         <v>449</v>
       </c>
-      <c r="J6" s="52">
+      <c r="J6" s="51">
         <v>2916</v>
       </c>
       <c r="K6" s="49">
@@ -25630,7 +25627,7 @@
       <c r="I7" s="49">
         <v>353</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="51">
         <v>6939</v>
       </c>
       <c r="K7" s="49">
@@ -25659,7 +25656,7 @@
       <c r="I8" s="49">
         <v>55</v>
       </c>
-      <c r="J8" s="52">
+      <c r="J8" s="51">
         <v>703</v>
       </c>
       <c r="K8" s="49">
@@ -25688,7 +25685,7 @@
       <c r="I9" s="49">
         <v>130</v>
       </c>
-      <c r="J9" s="52">
+      <c r="J9" s="51">
         <v>11250</v>
       </c>
       <c r="K9" s="49">
@@ -25717,7 +25714,7 @@
       <c r="I10" s="49">
         <v>45</v>
       </c>
-      <c r="J10" s="52">
+      <c r="J10" s="51">
         <v>861</v>
       </c>
       <c r="K10" s="49">
@@ -25746,7 +25743,7 @@
       <c r="I11" s="49">
         <v>7</v>
       </c>
-      <c r="J11" s="52">
+      <c r="J11" s="51">
         <v>486</v>
       </c>
       <c r="K11" s="49">
@@ -25775,7 +25772,7 @@
       <c r="I12" s="49">
         <v>1</v>
       </c>
-      <c r="J12" s="52">
+      <c r="J12" s="51">
         <v>252</v>
       </c>
       <c r="K12" s="49">
@@ -25804,7 +25801,7 @@
       <c r="I13" s="49">
         <v>1</v>
       </c>
-      <c r="J13" s="52">
+      <c r="J13" s="51">
         <v>369</v>
       </c>
       <c r="K13" s="49">
@@ -25833,7 +25830,7 @@
       <c r="I14" s="49">
         <v>22</v>
       </c>
-      <c r="J14" s="52">
+      <c r="J14" s="51">
         <v>234</v>
       </c>
       <c r="K14" s="49">
@@ -25862,7 +25859,7 @@
       <c r="I15" s="49">
         <v>23</v>
       </c>
-      <c r="J15" s="52">
+      <c r="J15" s="51">
         <v>450</v>
       </c>
       <c r="K15" s="49">
@@ -25891,7 +25888,7 @@
       <c r="I16" s="49">
         <v>21</v>
       </c>
-      <c r="J16" s="52">
+      <c r="J16" s="51">
         <v>338</v>
       </c>
       <c r="K16" s="49">
@@ -25920,7 +25917,7 @@
       <c r="I17" s="49">
         <v>54</v>
       </c>
-      <c r="J17" s="52">
+      <c r="J17" s="51">
         <v>3752</v>
       </c>
       <c r="K17" s="49">
@@ -25949,7 +25946,7 @@
       <c r="I18" s="49">
         <v>39</v>
       </c>
-      <c r="J18" s="52">
+      <c r="J18" s="51">
         <v>1511</v>
       </c>
       <c r="K18" s="49">
@@ -25978,7 +25975,7 @@
       <c r="I19" s="49">
         <v>20</v>
       </c>
-      <c r="J19" s="52">
+      <c r="J19" s="51">
         <v>528</v>
       </c>
       <c r="K19" s="49">
@@ -26006,7 +26003,7 @@
         <f>SUM(E2:E19)</f>
         <v>43020</v>
       </c>
-      <c r="H21" s="50" t="s">
+      <c r="H21" s="49" t="s">
         <v>155</v>
       </c>
       <c r="I21" s="49">
@@ -26045,8 +26042,8 @@
   <sheetPr/>
   <dimension ref="B1:Y76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -27005,8 +27002,8 @@
         <v>59</v>
       </c>
       <c r="L18" s="25">
-        <f>SUM(M17:Z17)</f>
-        <v>0</v>
+        <f>SUM(M18:U18)</f>
+        <v>84</v>
       </c>
       <c r="M18" s="25">
         <v>42</v>
@@ -27064,8 +27061,8 @@
         <v>64</v>
       </c>
       <c r="L19" s="25">
-        <f>SUM(M18:Z18)</f>
-        <v>84</v>
+        <f>SUM(M19:U19)</f>
+        <v>8831</v>
       </c>
       <c r="M19" s="25">
         <f t="shared" ref="M19:U19" si="4">SUM(M2:M16)</f>
@@ -30561,7 +30558,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{15dbf013-2542-44e2-b3cc-1b526430cc2b}</x14:id>
+          <x14:id>{079a5a5c-b479-4a3c-8a1b-fe8f7a80eb44}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30575,7 +30572,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{84c3a225-1bf9-47eb-bed7-81ca07cc0170}</x14:id>
+          <x14:id>{547cf61b-64a2-46c2-bfd5-fdb57d899f4b}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30589,7 +30586,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{79286149-106a-4ecd-98e2-706cc08fbc66}</x14:id>
+          <x14:id>{fb0db8bb-b697-4f4a-b4a8-dd77f85f1309}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30603,7 +30600,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1f3eef74-78b4-44a7-8d2c-a088496ea152}</x14:id>
+          <x14:id>{f3585e11-20c0-4634-b94e-0fe1645482fb}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30617,7 +30614,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{495a66d1-5922-458c-b2d1-d4a69fe804a9}</x14:id>
+          <x14:id>{1c39da72-31b1-42fb-8e84-7c49fbee63a3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30629,7 +30626,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ade4bdbe-536d-4e8d-ba92-3f2dc2fe1166}</x14:id>
+          <x14:id>{1c51fece-0efa-499d-9340-4b721e41017d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30643,7 +30640,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c094ff6a-aa05-4242-97bf-fac818fc248b}</x14:id>
+          <x14:id>{b7ec720a-082f-46ac-b740-00ef431130cc}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30657,7 +30654,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{64c9ea07-9112-4913-a971-2f3336ea3551}</x14:id>
+          <x14:id>{5e41a2b6-65d4-4f69-ad44-354ecd55b00b}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30669,7 +30666,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6a391b5b-a557-4337-9ef1-ab20e1d48793}</x14:id>
+          <x14:id>{e0fee39f-25d7-4731-ba5f-afb56fbd366c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30683,7 +30680,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{42674a29-82bc-4bb4-b88d-dace5105ad64}</x14:id>
+          <x14:id>{c453afd3-56a6-4966-8527-23430357cc3f}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30697,7 +30694,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f90929fc-e73c-4d6b-b0ab-fb801dc708e9}</x14:id>
+          <x14:id>{8dcc719f-b7fb-4ef0-892e-436a56fc7d9c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30709,7 +30706,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{dfa276bd-2f25-48c2-8f76-dec96122ff46}</x14:id>
+          <x14:id>{475cfaf4-e4fe-48e7-a60d-8eb5e6ba8b4d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30723,7 +30720,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{50dcd6bf-7529-4d78-a679-2c9ad668216f}</x14:id>
+          <x14:id>{05ddb806-875e-4c12-9ced-c4e896ca8f08}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30735,7 +30732,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3e258eeb-e998-4182-9e0f-680e7cc5efa5}</x14:id>
+          <x14:id>{67c47bae-3382-4c12-84b3-6b5c973451fe}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30747,7 +30744,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{35c16876-edcb-4624-a520-80f1ef8a0a77}</x14:id>
+          <x14:id>{b199af65-3190-4c72-b187-1a35f879e1cb}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30761,7 +30758,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{011b9680-12b7-441f-b840-c478f3b803fa}</x14:id>
+          <x14:id>{8debb382-1ccb-460c-b27f-b8740f05cc03}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30773,7 +30770,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{446609e5-6e25-439f-86a0-f8dc8dc2d640}</x14:id>
+          <x14:id>{edc7167b-84e9-4490-af24-dc2a18771c23}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30785,7 +30782,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7099b419-bde3-4d0e-a198-842fb4009477}</x14:id>
+          <x14:id>{22f40229-7942-49c0-ac69-c5196317a559}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30799,7 +30796,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{d49276e6-d3ae-485a-996e-a7e73c4b63ad}</x14:id>
+          <x14:id>{8d7bb226-b3f3-4459-946d-c9ff0a69d0a1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30811,7 +30808,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{d41ef250-b3bc-422f-bafc-b2134d283ee7}</x14:id>
+          <x14:id>{8e43a9c9-6ede-491d-958b-e0630b013812}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30823,7 +30820,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{995e750f-af99-4ac6-ab01-2ba46f34383f}</x14:id>
+          <x14:id>{505f202d-2fae-4600-ba11-3e6ed45c810f}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -30834,7 +30831,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{15dbf013-2542-44e2-b3cc-1b526430cc2b}">
+          <x14:cfRule type="dataBar" id="{079a5a5c-b479-4a3c-8a1b-fe8f7a80eb44}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30847,7 +30844,7 @@
           <xm:sqref>G22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{84c3a225-1bf9-47eb-bed7-81ca07cc0170}">
+          <x14:cfRule type="dataBar" id="{547cf61b-64a2-46c2-bfd5-fdb57d899f4b}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30860,7 +30857,7 @@
           <xm:sqref>G45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{79286149-106a-4ecd-98e2-706cc08fbc66}">
+          <x14:cfRule type="dataBar" id="{fb0db8bb-b697-4f4a-b4a8-dd77f85f1309}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30873,7 +30870,7 @@
           <xm:sqref>G69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1f3eef74-78b4-44a7-8d2c-a088496ea152}">
+          <x14:cfRule type="dataBar" id="{f3585e11-20c0-4634-b94e-0fe1645482fb}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30884,7 +30881,7 @@
           <xm:sqref>G8:G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{495a66d1-5922-458c-b2d1-d4a69fe804a9}">
+          <x14:cfRule type="dataBar" id="{1c39da72-31b1-42fb-8e84-7c49fbee63a3}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -30896,7 +30893,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{ade4bdbe-536d-4e8d-ba92-3f2dc2fe1166}">
+          <x14:cfRule type="dataBar" id="{1c51fece-0efa-499d-9340-4b721e41017d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30909,7 +30906,7 @@
           <xm:sqref>G8:G22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c094ff6a-aa05-4242-97bf-fac818fc248b}">
+          <x14:cfRule type="dataBar" id="{b7ec720a-082f-46ac-b740-00ef431130cc}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30920,7 +30917,7 @@
           <xm:sqref>G31:G44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{64c9ea07-9112-4913-a971-2f3336ea3551}">
+          <x14:cfRule type="dataBar" id="{5e41a2b6-65d4-4f69-ad44-354ecd55b00b}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -30932,7 +30929,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{6a391b5b-a557-4337-9ef1-ab20e1d48793}">
+          <x14:cfRule type="dataBar" id="{e0fee39f-25d7-4731-ba5f-afb56fbd366c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30945,7 +30942,7 @@
           <xm:sqref>G31:G45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{42674a29-82bc-4bb4-b88d-dace5105ad64}">
+          <x14:cfRule type="dataBar" id="{c453afd3-56a6-4966-8527-23430357cc3f}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30956,7 +30953,7 @@
           <xm:sqref>G55:G68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f90929fc-e73c-4d6b-b0ab-fb801dc708e9}">
+          <x14:cfRule type="dataBar" id="{8dcc719f-b7fb-4ef0-892e-436a56fc7d9c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -30966,7 +30963,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{dfa276bd-2f25-48c2-8f76-dec96122ff46}">
+          <x14:cfRule type="dataBar" id="{475cfaf4-e4fe-48e7-a60d-8eb5e6ba8b4d}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -30981,7 +30978,7 @@
           <xm:sqref>G55:G69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{50dcd6bf-7529-4d78-a679-2c9ad668216f}">
+          <x14:cfRule type="dataBar" id="{05ddb806-875e-4c12-9ced-c4e896ca8f08}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -30993,7 +30990,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{3e258eeb-e998-4182-9e0f-680e7cc5efa5}">
+          <x14:cfRule type="dataBar" id="{67c47bae-3382-4c12-84b3-6b5c973451fe}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -31005,7 +31002,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{35c16876-edcb-4624-a520-80f1ef8a0a77}">
+          <x14:cfRule type="dataBar" id="{b199af65-3190-4c72-b187-1a35f879e1cb}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -31016,7 +31013,7 @@
           <xm:sqref>H4:H22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{011b9680-12b7-441f-b840-c478f3b803fa}">
+          <x14:cfRule type="dataBar" id="{8debb382-1ccb-460c-b27f-b8740f05cc03}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -31028,7 +31025,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{446609e5-6e25-439f-86a0-f8dc8dc2d640}">
+          <x14:cfRule type="dataBar" id="{edc7167b-84e9-4490-af24-dc2a18771c23}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -31040,7 +31037,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{7099b419-bde3-4d0e-a198-842fb4009477}">
+          <x14:cfRule type="dataBar" id="{22f40229-7942-49c0-ac69-c5196317a559}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -31051,7 +31048,7 @@
           <xm:sqref>H27:H45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{d49276e6-d3ae-485a-996e-a7e73c4b63ad}">
+          <x14:cfRule type="dataBar" id="{8d7bb226-b3f3-4459-946d-c9ff0a69d0a1}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -31059,7 +31056,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{d41ef250-b3bc-422f-bafc-b2134d283ee7}">
+          <x14:cfRule type="dataBar" id="{8e43a9c9-6ede-491d-958b-e0630b013812}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -31071,7 +31068,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{995e750f-af99-4ac6-ab01-2ba46f34383f}">
+          <x14:cfRule type="dataBar" id="{505f202d-2fae-4600-ba11-3e6ed45c810f}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>